<commit_message>
Fix implied volatility inconsistencies and writeRealtime fixes
</commit_message>
<xml_diff>
--- a/data/options-recap/realtime/excel/Options Recap.xlsx
+++ b/data/options-recap/realtime/excel/Options Recap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Programming\Cue\data\options-recap\realtime\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A27A39-F3FB-457E-A01F-F080460F14A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08B1285-62AB-449D-B320-1D235BD4B742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{46699434-473C-4966-BCFA-04206E4C53EA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="355">
   <si>
     <t>Ticker</t>
   </si>
@@ -111,9 +111,6 @@
     <t>Call</t>
   </si>
   <si>
-    <t>OKAY|1</t>
-  </si>
-  <si>
     <t>XLF</t>
   </si>
   <si>
@@ -174,15 +171,9 @@
     <t>SPY</t>
   </si>
   <si>
-    <t>BEST|30420</t>
-  </si>
-  <si>
     <t>OKAY|30</t>
   </si>
   <si>
-    <t>OKAY|39.5</t>
-  </si>
-  <si>
     <t>BAD|42.41</t>
   </si>
   <si>
@@ -198,333 +189,87 @@
     <t>|0</t>
   </si>
   <si>
-    <t>OKAY|-0.1916</t>
-  </si>
-  <si>
-    <t>GOOD|0.0751</t>
-  </si>
-  <si>
-    <t>OKAY|0.0339</t>
-  </si>
-  <si>
-    <t>OKAY|-0.0158</t>
-  </si>
-  <si>
-    <t>BAD|-0.7304</t>
-  </si>
-  <si>
-    <t>BEST|0.43</t>
-  </si>
-  <si>
-    <t>OKAY|30720</t>
-  </si>
-  <si>
-    <t>BEST|37</t>
-  </si>
-  <si>
     <t>OKAY|12.5</t>
   </si>
   <si>
-    <t>BAD|9.99</t>
-  </si>
-  <si>
-    <t>BAD|2234</t>
-  </si>
-  <si>
-    <t>BAD|3</t>
-  </si>
-  <si>
     <t>OKAY|744.6666666666666</t>
   </si>
   <si>
-    <t>BEST|0.1904</t>
-  </si>
-  <si>
-    <t>GOOD|0.0591</t>
-  </si>
-  <si>
-    <t>OKAY|0.0081</t>
-  </si>
-  <si>
     <t>BAD|-0.0049</t>
   </si>
   <si>
     <t>BAD|0.1585</t>
   </si>
   <si>
-    <t>BEST|0.5</t>
-  </si>
-  <si>
-    <t>BAD|31500</t>
-  </si>
-  <si>
     <t>OKAY|16</t>
   </si>
   <si>
     <t>OKAY|36</t>
   </si>
   <si>
-    <t>OKAY|38.06</t>
-  </si>
-  <si>
     <t>BAD|-5.412506568575937</t>
   </si>
   <si>
     <t>BAD|12449</t>
   </si>
   <si>
-    <t>BEST|216</t>
-  </si>
-  <si>
     <t>BAD|57.63425925925926</t>
   </si>
   <si>
     <t>BAD|-0.1576</t>
   </si>
   <si>
-    <t>BAD|0.1167</t>
-  </si>
-  <si>
-    <t>GOOD|0.0199</t>
-  </si>
-  <si>
-    <t>OKAY|-0.0153</t>
-  </si>
-  <si>
-    <t>BAD|-0.2918</t>
-  </si>
-  <si>
-    <t>GOOD|0.18</t>
-  </si>
-  <si>
-    <t>BAD|32580</t>
-  </si>
-  <si>
-    <t>OKAY|76</t>
-  </si>
-  <si>
     <t>OKAY|72.09</t>
   </si>
   <si>
-    <t>GOOD|4625</t>
-  </si>
-  <si>
-    <t>OKAY|20</t>
-  </si>
-  <si>
-    <t>BAD|231.25</t>
-  </si>
-  <si>
     <t>GOOD|0.1643</t>
   </si>
   <si>
-    <t>OKAY|0.0644</t>
-  </si>
-  <si>
-    <t>GOOD|0.0577</t>
-  </si>
-  <si>
-    <t>GOOD|-0.0124</t>
-  </si>
-  <si>
     <t>OKAY|1.2056</t>
   </si>
   <si>
-    <t>BAD|0.35</t>
-  </si>
-  <si>
-    <t>OKAY|32700</t>
-  </si>
-  <si>
     <t>OKAY|14.5</t>
   </si>
   <si>
-    <t>BAD|13.71</t>
-  </si>
-  <si>
-    <t>GOOD|400</t>
-  </si>
-  <si>
-    <t>GOOD|133.33333333333334</t>
-  </si>
-  <si>
     <t>BAD|0.438</t>
   </si>
   <si>
-    <t>BAD|0.1383</t>
-  </si>
-  <si>
-    <t>OKAY|0.0159</t>
-  </si>
-  <si>
-    <t>BAD|-0.0176</t>
-  </si>
-  <si>
     <t>BEST|0.4459</t>
   </si>
   <si>
-    <t>BEST|0.9</t>
-  </si>
-  <si>
-    <t>GOOD|33900</t>
-  </si>
-  <si>
     <t>OKAY|104.5</t>
   </si>
   <si>
-    <t>OKAY|109.78</t>
-  </si>
-  <si>
-    <t>BAD|-4.809619238476959</t>
-  </si>
-  <si>
-    <t>BEST|1275</t>
-  </si>
-  <si>
-    <t>OKAY|5</t>
-  </si>
-  <si>
-    <t>OKAY|255</t>
-  </si>
-  <si>
-    <t>OKAY|-0.1557</t>
-  </si>
-  <si>
     <t>OKAY|0.0473</t>
   </si>
   <si>
-    <t>BEST|0.0569</t>
-  </si>
-  <si>
-    <t>OKAY|-0.0387</t>
-  </si>
-  <si>
-    <t>BAD|-0.8265</t>
-  </si>
-  <si>
-    <t>GOOD|0.44</t>
-  </si>
-  <si>
-    <t>OKAY|34440</t>
-  </si>
-  <si>
     <t>OKAY|9</t>
   </si>
   <si>
-    <t>BAD|50.5</t>
-  </si>
-  <si>
-    <t>GOOD|48.06</t>
-  </si>
-  <si>
-    <t>BAD|3074</t>
-  </si>
-  <si>
     <t>OKAY|460</t>
   </si>
   <si>
-    <t>OKAY|6.682608695652174</t>
-  </si>
-  <si>
-    <t>GOOD|0.1976</t>
-  </si>
-  <si>
-    <t>BAD|0.1027</t>
-  </si>
-  <si>
-    <t>BAD|0.0224</t>
-  </si>
-  <si>
     <t>OKAY|-0.0366</t>
   </si>
   <si>
-    <t>BAD|0.2578</t>
-  </si>
-  <si>
-    <t>OKAY|0.3</t>
-  </si>
-  <si>
-    <t>GOOD|34980</t>
-  </si>
-  <si>
-    <t>OKAY|44</t>
-  </si>
-  <si>
-    <t>BAD|80</t>
-  </si>
-  <si>
-    <t>BAD|62.31</t>
-  </si>
-  <si>
-    <t>OKAY|263</t>
-  </si>
-  <si>
-    <t>BAD|263</t>
-  </si>
-  <si>
     <t>BAD|0.1069</t>
   </si>
   <si>
     <t>OKAY|0.0158</t>
   </si>
   <si>
-    <t>BAD|0.0404</t>
-  </si>
-  <si>
     <t>OKAY|-0.0238</t>
   </si>
   <si>
-    <t>GOOD|0.756</t>
-  </si>
-  <si>
-    <t>BAD|0.6</t>
-  </si>
-  <si>
-    <t>OKAY|35640</t>
-  </si>
-  <si>
     <t>GOOD|72</t>
   </si>
   <si>
-    <t>GOOD|32</t>
-  </si>
-  <si>
     <t>OKAY|36.48</t>
   </si>
   <si>
-    <t>GOOD|-12.280701754385959</t>
-  </si>
-  <si>
-    <t>OKAY|582</t>
-  </si>
-  <si>
     <t>BEST|194</t>
   </si>
   <si>
-    <t>BAD|-0.1999</t>
-  </si>
-  <si>
-    <t>BAD|0.0444</t>
-  </si>
-  <si>
-    <t>GOOD|0.0457</t>
-  </si>
-  <si>
-    <t>OKAY|-0.0121</t>
-  </si>
-  <si>
-    <t>BEST|-1.6171</t>
-  </si>
-  <si>
-    <t>OKAY|0.78</t>
-  </si>
-  <si>
-    <t>BAD|35880</t>
-  </si>
-  <si>
-    <t>BAD|7.5</t>
-  </si>
-  <si>
     <t>GOOD|6.41</t>
   </si>
   <si>
@@ -534,126 +279,45 @@
     <t>BAD|822</t>
   </si>
   <si>
-    <t>BAD|8.177615571776157</t>
-  </si>
-  <si>
-    <t>OKAY|0.4019</t>
-  </si>
-  <si>
-    <t>GOOD|0.1428</t>
-  </si>
-  <si>
     <t>OKAY|0.0079</t>
   </si>
   <si>
-    <t>OKAY|-0.0115</t>
-  </si>
-  <si>
-    <t>BAD|0.2066</t>
-  </si>
-  <si>
-    <t>OKAY|0.65</t>
-  </si>
-  <si>
-    <t>BAD|36480</t>
-  </si>
-  <si>
-    <t>BAD|8</t>
-  </si>
-  <si>
     <t>BAD|7.22</t>
   </si>
   <si>
-    <t>OKAY|379</t>
-  </si>
-  <si>
-    <t>GOOD|42</t>
-  </si>
-  <si>
-    <t>GOOD|9.023809523809524</t>
-  </si>
-  <si>
-    <t>BEST|0.3642</t>
-  </si>
-  <si>
-    <t>BAD|0.2258</t>
-  </si>
-  <si>
-    <t>BEST|0.0095</t>
-  </si>
-  <si>
-    <t>GOOD|-0.0067</t>
-  </si>
-  <si>
     <t>BAD|0.2804</t>
   </si>
   <si>
-    <t>OKAY|0.38</t>
-  </si>
-  <si>
-    <t>OKAY|37980</t>
-  </si>
-  <si>
     <t>OKAY|7.09</t>
   </si>
   <si>
     <t>GOOD|41.000000000000014</t>
   </si>
   <si>
-    <t>BEST|3235</t>
-  </si>
-  <si>
-    <t>GOOD|421</t>
-  </si>
-  <si>
     <t>BAD|7.684085510688836</t>
   </si>
   <si>
     <t>GOOD|-0.5764</t>
   </si>
   <si>
-    <t>BEST|0.2597</t>
-  </si>
-  <si>
-    <t>OKAY|0.0046</t>
-  </si>
-  <si>
     <t>OKAY|-0.0318</t>
   </si>
   <si>
     <t>OKAY|-0.1383</t>
   </si>
   <si>
-    <t>GOOD|40080</t>
-  </si>
-  <si>
-    <t>GOOD|23</t>
-  </si>
-  <si>
     <t>OKAY|58</t>
   </si>
   <si>
     <t>GOOD|54.69</t>
   </si>
   <si>
-    <t>OKAY|3735</t>
-  </si>
-  <si>
     <t>OKAY|587</t>
   </si>
   <si>
-    <t>BAD|6.362862010221465</t>
-  </si>
-  <si>
     <t>BAD|0.1968</t>
   </si>
   <si>
-    <t>OKAY|0.0764</t>
-  </si>
-  <si>
-    <t>BEST|0.039</t>
-  </si>
-  <si>
     <t>OKAY|-0.0208</t>
   </si>
   <si>
@@ -666,9 +330,6 @@
     <t>BAD|40620</t>
   </si>
   <si>
-    <t>BEST|41</t>
-  </si>
-  <si>
     <t>OKAY|36.34</t>
   </si>
   <si>
@@ -678,45 +339,9 @@
     <t>BAD|1789</t>
   </si>
   <si>
-    <t>GOOD|3.413638904415875</t>
-  </si>
-  <si>
-    <t>OKAY|0.1135</t>
-  </si>
-  <si>
-    <t>BAD|0.0553</t>
-  </si>
-  <si>
-    <t>OKAY|0.0226</t>
-  </si>
-  <si>
-    <t>GOOD|-0.0088</t>
-  </si>
-  <si>
     <t>BAD|0.4122</t>
   </si>
   <si>
-    <t>BAD|0.19</t>
-  </si>
-  <si>
-    <t>BAD|42120</t>
-  </si>
-  <si>
-    <t>GOOD|5.5</t>
-  </si>
-  <si>
-    <t>GOOD|5.05</t>
-  </si>
-  <si>
-    <t>BEST|45.000000000000014</t>
-  </si>
-  <si>
-    <t>BAD|3115</t>
-  </si>
-  <si>
-    <t>BEST|569</t>
-  </si>
-  <si>
     <t>OKAY|5.474516695957821</t>
   </si>
   <si>
@@ -726,12 +351,6 @@
     <t>BAD|0.383</t>
   </si>
   <si>
-    <t>OKAY|0.0061</t>
-  </si>
-  <si>
-    <t>GOOD|-0.0047</t>
-  </si>
-  <si>
     <t>BEST|0.1656</t>
   </si>
   <si>
@@ -741,39 +360,18 @@
     <t>GOOD|43020</t>
   </si>
   <si>
-    <t>OKAY|135</t>
-  </si>
-  <si>
-    <t>GOOD|9.25</t>
-  </si>
-  <si>
     <t>BAD|15035</t>
   </si>
   <si>
     <t>BEST|391</t>
   </si>
   <si>
-    <t>BAD|38.452685421994886</t>
-  </si>
-  <si>
-    <t>BEST|0.1373</t>
-  </si>
-  <si>
     <t>OKAY|0.0922</t>
   </si>
   <si>
-    <t>BEST|0.0124</t>
-  </si>
-  <si>
-    <t>GOOD|-0.0018</t>
-  </si>
-  <si>
     <t>OKAY|0.4185</t>
   </si>
   <si>
-    <t>BAD|0.2</t>
-  </si>
-  <si>
     <t>BAD|43200</t>
   </si>
   <si>
@@ -783,141 +381,63 @@
     <t>BAD|84.07</t>
   </si>
   <si>
-    <t>BEST|564</t>
-  </si>
-  <si>
     <t>BAD|24</t>
   </si>
   <si>
     <t>OKAY|23.5</t>
   </si>
   <si>
-    <t>GOOD|0.1143</t>
-  </si>
-  <si>
     <t>OKAY|0.0131</t>
   </si>
   <si>
     <t>OKAY|0.0727</t>
   </si>
   <si>
-    <t>BAD|-0.0189</t>
-  </si>
-  <si>
-    <t>OKAY|1.7741</t>
-  </si>
-  <si>
     <t>GOOD|0.79</t>
   </si>
   <si>
-    <t>BAD|43860</t>
-  </si>
-  <si>
-    <t>BEST|2</t>
-  </si>
-  <si>
     <t>GOOD|33.5</t>
   </si>
   <si>
-    <t>BAD|31.8</t>
-  </si>
-  <si>
-    <t>GOOD|1954</t>
-  </si>
-  <si>
     <t>GOOD|80</t>
   </si>
   <si>
     <t>OKAY|24.425</t>
   </si>
   <si>
-    <t>OKAY|0.3344</t>
-  </si>
-  <si>
-    <t>OKAY|0.1057</t>
-  </si>
-  <si>
-    <t>OKAY|0.0107</t>
-  </si>
-  <si>
-    <t>OKAY|-0.2017</t>
-  </si>
-  <si>
-    <t>OKAY|0.0845</t>
-  </si>
-  <si>
     <t>OKAY|0.74</t>
   </si>
   <si>
-    <t>BAD|43980</t>
-  </si>
-  <si>
-    <t>BAD|230</t>
-  </si>
-  <si>
     <t>BAD|206.43</t>
   </si>
   <si>
-    <t>BEST|1034</t>
-  </si>
-  <si>
     <t>BAD|1034</t>
   </si>
   <si>
-    <t>BAD|0.0706</t>
-  </si>
-  <si>
     <t>OKAY|0.0089</t>
   </si>
   <si>
-    <t>BEST|0.0981</t>
-  </si>
-  <si>
     <t>OKAY|-0.022</t>
   </si>
   <si>
     <t>OKAY|1.745</t>
   </si>
   <si>
-    <t>OKAY|0.51</t>
-  </si>
-  <si>
-    <t>OKAY|46800</t>
-  </si>
-  <si>
     <t>OKAY|6</t>
   </si>
   <si>
-    <t>GOOD|8.16</t>
-  </si>
-  <si>
     <t>BAD|-26.470588235294123</t>
   </si>
   <si>
     <t>GOOD|442</t>
   </si>
   <si>
-    <t>OKAY|68</t>
-  </si>
-  <si>
     <t>BAD|6.5</t>
   </si>
   <si>
-    <t>OKAY|-0.218</t>
-  </si>
-  <si>
-    <t>BEST|0.0609</t>
-  </si>
-  <si>
-    <t>OKAY|0.0051</t>
-  </si>
-  <si>
     <t>OKAY|-0.0448</t>
   </si>
   <si>
-    <t>BAD|-0.122</t>
-  </si>
-  <si>
     <t>BAD|47340</t>
   </si>
   <si>
@@ -927,81 +447,30 @@
     <t>BAD|31</t>
   </si>
   <si>
-    <t>BAD|24.59</t>
-  </si>
-  <si>
-    <t>GOOD|432</t>
-  </si>
-  <si>
-    <t>GOOD|21.6</t>
-  </si>
-  <si>
     <t>OKAY|0.1633</t>
   </si>
   <si>
-    <t>GOOD|0.0433</t>
-  </si>
-  <si>
-    <t>BEST|0.0467</t>
-  </si>
-  <si>
     <t>OKAY|-0.0028</t>
   </si>
   <si>
     <t>OKAY|2.1443</t>
   </si>
   <si>
-    <t>BEST|0.46</t>
-  </si>
-  <si>
     <t>BAD|47820</t>
   </si>
   <si>
-    <t>BEST|38</t>
-  </si>
-  <si>
     <t>BAD|42.01</t>
   </si>
   <si>
-    <t>BAD|-9.545346346108063</t>
-  </si>
-  <si>
-    <t>GOOD|595</t>
-  </si>
-  <si>
-    <t>GOOD|150</t>
-  </si>
-  <si>
-    <t>BAD|3.966666666666667</t>
-  </si>
-  <si>
-    <t>BAD|-0.1411</t>
-  </si>
-  <si>
     <t>OKAY|0.0543</t>
   </si>
   <si>
-    <t>BEST|0.0156</t>
-  </si>
-  <si>
-    <t>OKAY|-0.0458</t>
-  </si>
-  <si>
-    <t>BAD|-0.172</t>
-  </si>
-  <si>
     <t>GOOD|0.32</t>
   </si>
   <si>
-    <t>OKAY|50040</t>
-  </si>
-  <si>
     <t>BAD|5</t>
   </si>
   <si>
-    <t>OKAY|390</t>
-  </si>
-  <si>
     <t>OKAY|451.79</t>
   </si>
   <si>
@@ -1011,28 +480,625 @@
     <t>BAD|11521</t>
   </si>
   <si>
-    <t>GOOD|153</t>
-  </si>
-  <si>
     <t>BAD|75.30065359477125</t>
   </si>
   <si>
-    <t>BAD|-0.0043</t>
-  </si>
-  <si>
-    <t>BAD|0.0005</t>
-  </si>
-  <si>
     <t>BEST|0.0073</t>
   </si>
   <si>
-    <t>BAD|-0.0267</t>
-  </si>
-  <si>
     <t>BAD|-0.0325</t>
   </si>
   <si>
-    <t>GOOD|0.04</t>
+    <t>BAD|30420</t>
+  </si>
+  <si>
+    <t>GOOD|39.5</t>
+  </si>
+  <si>
+    <t>GOOD|1</t>
+  </si>
+  <si>
+    <t>OKAY|0.2926</t>
+  </si>
+  <si>
+    <t>BAD|-0.1916</t>
+  </si>
+  <si>
+    <t>BEST|0.0751</t>
+  </si>
+  <si>
+    <t>GOOD|0.0339</t>
+  </si>
+  <si>
+    <t>GOOD|-0.0158</t>
+  </si>
+  <si>
+    <t>GOOD|-0.7304</t>
+  </si>
+  <si>
+    <t>BAD|0.43</t>
+  </si>
+  <si>
+    <t>BAD|30720</t>
+  </si>
+  <si>
+    <t>OKAY|37</t>
+  </si>
+  <si>
+    <t>GOOD|9.99</t>
+  </si>
+  <si>
+    <t>OKAY|2234</t>
+  </si>
+  <si>
+    <t>OKAY|3</t>
+  </si>
+  <si>
+    <t>OKAY|1.319</t>
+  </si>
+  <si>
+    <t>BAD|0.1904</t>
+  </si>
+  <si>
+    <t>OKAY|0.0591</t>
+  </si>
+  <si>
+    <t>BAD|0.0081</t>
+  </si>
+  <si>
+    <t>OKAY|0.5</t>
+  </si>
+  <si>
+    <t>GOOD|31500</t>
+  </si>
+  <si>
+    <t>BAD|38.06</t>
+  </si>
+  <si>
+    <t>BAD|216</t>
+  </si>
+  <si>
+    <t>BAD|0.2494</t>
+  </si>
+  <si>
+    <t>OKAY|0.1167</t>
+  </si>
+  <si>
+    <t>BEST|0.0199</t>
+  </si>
+  <si>
+    <t>BEST|-0.0153</t>
+  </si>
+  <si>
+    <t>BEST|-0.2918</t>
+  </si>
+  <si>
+    <t>BEST|0.18</t>
+  </si>
+  <si>
+    <t>OKAY|32580</t>
+  </si>
+  <si>
+    <t>BAD|76</t>
+  </si>
+  <si>
+    <t>BAD|4625</t>
+  </si>
+  <si>
+    <t>BAD|20</t>
+  </si>
+  <si>
+    <t>OKAY|231.25</t>
+  </si>
+  <si>
+    <t>BAD|0.1648</t>
+  </si>
+  <si>
+    <t>BAD|0.0644</t>
+  </si>
+  <si>
+    <t>OKAY|0.0577</t>
+  </si>
+  <si>
+    <t>OKAY|-0.0124</t>
+  </si>
+  <si>
+    <t>OKAY|0.35</t>
+  </si>
+  <si>
+    <t>BAD|32700</t>
+  </si>
+  <si>
+    <t>OKAY|13.71</t>
+  </si>
+  <si>
+    <t>BAD|400</t>
+  </si>
+  <si>
+    <t>BAD|133.33333333333334</t>
+  </si>
+  <si>
+    <t>GOOD|0.7059000000000001</t>
+  </si>
+  <si>
+    <t>OKAY|0.1383</t>
+  </si>
+  <si>
+    <t>BAD|0.0159</t>
+  </si>
+  <si>
+    <t>OKAY|-0.0176</t>
+  </si>
+  <si>
+    <t>OKAY|0.9</t>
+  </si>
+  <si>
+    <t>BAD|33900</t>
+  </si>
+  <si>
+    <t>GOOD|109.78</t>
+  </si>
+  <si>
+    <t>OKAY|-4.809619238476959</t>
+  </si>
+  <si>
+    <t>OKAY|1275</t>
+  </si>
+  <si>
+    <t>GOOD|5</t>
+  </si>
+  <si>
+    <t>BAD|255</t>
+  </si>
+  <si>
+    <t>BAD|0.21170000000000003</t>
+  </si>
+  <si>
+    <t>BEST|-0.1557</t>
+  </si>
+  <si>
+    <t>OKAY|0.0569</t>
+  </si>
+  <si>
+    <t>BAD|-0.0387</t>
+  </si>
+  <si>
+    <t>OKAY|-0.8265</t>
+  </si>
+  <si>
+    <t>OKAY|0.44</t>
+  </si>
+  <si>
+    <t>BEST|34440</t>
+  </si>
+  <si>
+    <t>OKAY|50.5</t>
+  </si>
+  <si>
+    <t>OKAY|48.06</t>
+  </si>
+  <si>
+    <t>OKAY|3074</t>
+  </si>
+  <si>
+    <t>BEST|6.682608695652174</t>
+  </si>
+  <si>
+    <t>OKAY|0.33630000000000004</t>
+  </si>
+  <si>
+    <t>BAD|0.1976</t>
+  </si>
+  <si>
+    <t>OKAY|0.1027</t>
+  </si>
+  <si>
+    <t>GOOD|0.0224</t>
+  </si>
+  <si>
+    <t>OKAY|0.2578</t>
+  </si>
+  <si>
+    <t>BEST|0.3</t>
+  </si>
+  <si>
+    <t>OKAY|34980</t>
+  </si>
+  <si>
+    <t>GOOD|44</t>
+  </si>
+  <si>
+    <t>OKAY|80</t>
+  </si>
+  <si>
+    <t>GOOD|62.31</t>
+  </si>
+  <si>
+    <t>GOOD|263</t>
+  </si>
+  <si>
+    <t>BAD|0.5324</t>
+  </si>
+  <si>
+    <t>OKAY|0.0404</t>
+  </si>
+  <si>
+    <t>BAD|0.756</t>
+  </si>
+  <si>
+    <t>OKAY|0.6</t>
+  </si>
+  <si>
+    <t>BAD|35640</t>
+  </si>
+  <si>
+    <t>BAD|32</t>
+  </si>
+  <si>
+    <t>BAD|-12.280701754385959</t>
+  </si>
+  <si>
+    <t>GOOD|582</t>
+  </si>
+  <si>
+    <t>BEST|0.38539999999999996</t>
+  </si>
+  <si>
+    <t>OKAY|-0.1999</t>
+  </si>
+  <si>
+    <t>OKAY|0.0444</t>
+  </si>
+  <si>
+    <t>BEST|0.0457</t>
+  </si>
+  <si>
+    <t>GOOD|-0.0121</t>
+  </si>
+  <si>
+    <t>BAD|-1.6171</t>
+  </si>
+  <si>
+    <t>GOOD|0.78</t>
+  </si>
+  <si>
+    <t>GOOD|35880</t>
+  </si>
+  <si>
+    <t>OKAY|7.5</t>
+  </si>
+  <si>
+    <t>GOOD|8.177615571776157</t>
+  </si>
+  <si>
+    <t>BAD|1.2736</t>
+  </si>
+  <si>
+    <t>BAD|0.4019</t>
+  </si>
+  <si>
+    <t>OKAY|0.1428</t>
+  </si>
+  <si>
+    <t>GOOD|-0.0115</t>
+  </si>
+  <si>
+    <t>BEST|0.2066</t>
+  </si>
+  <si>
+    <t>BAD|0.65</t>
+  </si>
+  <si>
+    <t>GOOD|36480</t>
+  </si>
+  <si>
+    <t>OKAY|8</t>
+  </si>
+  <si>
+    <t>GOOD|379</t>
+  </si>
+  <si>
+    <t>BAD|42</t>
+  </si>
+  <si>
+    <t>BAD|9.023809523809524</t>
+  </si>
+  <si>
+    <t>OKAY|0.6527</t>
+  </si>
+  <si>
+    <t>GOOD|0.3642</t>
+  </si>
+  <si>
+    <t>GOOD|0.2258</t>
+  </si>
+  <si>
+    <t>GOOD|0.0095</t>
+  </si>
+  <si>
+    <t>OKAY|-0.0067</t>
+  </si>
+  <si>
+    <t>GOOD|0.38</t>
+  </si>
+  <si>
+    <t>GOOD|37980</t>
+  </si>
+  <si>
+    <t>BAD|3235</t>
+  </si>
+  <si>
+    <t>OKAY|421</t>
+  </si>
+  <si>
+    <t>OKAY|1.2604</t>
+  </si>
+  <si>
+    <t>BAD|0.2597</t>
+  </si>
+  <si>
+    <t>BAD|0.0046</t>
+  </si>
+  <si>
+    <t>BEST|40080</t>
+  </si>
+  <si>
+    <t>OKAY|23</t>
+  </si>
+  <si>
+    <t>GOOD|3735</t>
+  </si>
+  <si>
+    <t>OKAY|6.362862010221465</t>
+  </si>
+  <si>
+    <t>OKAY|0.258</t>
+  </si>
+  <si>
+    <t>GOOD|0.0764</t>
+  </si>
+  <si>
+    <t>OKAY|0.039</t>
+  </si>
+  <si>
+    <t>OKAY|41</t>
+  </si>
+  <si>
+    <t>BAD|3.413638904415875</t>
+  </si>
+  <si>
+    <t>OKAY|0.2961</t>
+  </si>
+  <si>
+    <t>BAD|0.1135</t>
+  </si>
+  <si>
+    <t>GOOD|0.0553</t>
+  </si>
+  <si>
+    <t>GOOD|0.0226</t>
+  </si>
+  <si>
+    <t>OKAY|-0.0088</t>
+  </si>
+  <si>
+    <t>GOOD|0.19</t>
+  </si>
+  <si>
+    <t>OKAY|42120</t>
+  </si>
+  <si>
+    <t>OKAY|5.5</t>
+  </si>
+  <si>
+    <t>BEST|5.05</t>
+  </si>
+  <si>
+    <t>OKAY|45.000000000000014</t>
+  </si>
+  <si>
+    <t>OKAY|3115</t>
+  </si>
+  <si>
+    <t>BAD|569</t>
+  </si>
+  <si>
+    <t>BAD|0.5981000000000001</t>
+  </si>
+  <si>
+    <t>BAD|0.0061</t>
+  </si>
+  <si>
+    <t>OKAY|-0.0047</t>
+  </si>
+  <si>
+    <t>GOOD|135</t>
+  </si>
+  <si>
+    <t>BAD|9.25</t>
+  </si>
+  <si>
+    <t>GOOD|38.452685421994886</t>
+  </si>
+  <si>
+    <t>GOOD|0.41979999999999995</t>
+  </si>
+  <si>
+    <t>BAD|0.1373</t>
+  </si>
+  <si>
+    <t>OKAY|0.0124</t>
+  </si>
+  <si>
+    <t>OKAY|-0.0018</t>
+  </si>
+  <si>
+    <t>OKAY|0.2</t>
+  </si>
+  <si>
+    <t>OKAY|564</t>
+  </si>
+  <si>
+    <t>OKAY|0.39149999999999996</t>
+  </si>
+  <si>
+    <t>BAD|0.1143</t>
+  </si>
+  <si>
+    <t>OKAY|-0.0189</t>
+  </si>
+  <si>
+    <t>GOOD|1.7741</t>
+  </si>
+  <si>
+    <t>OKAY|43860</t>
+  </si>
+  <si>
+    <t>GOOD|2</t>
+  </si>
+  <si>
+    <t>OKAY|31.8</t>
+  </si>
+  <si>
+    <t>BEST|1954</t>
+  </si>
+  <si>
+    <t>BAD|1.1739</t>
+  </si>
+  <si>
+    <t>BEST|0.3344</t>
+  </si>
+  <si>
+    <t>GOOD|0.1057</t>
+  </si>
+  <si>
+    <t>BAD|0.0107</t>
+  </si>
+  <si>
+    <t>GOOD|-0.2017</t>
+  </si>
+  <si>
+    <t>GOOD|0.0845</t>
+  </si>
+  <si>
+    <t>GOOD|43980</t>
+  </si>
+  <si>
+    <t>BEST|230</t>
+  </si>
+  <si>
+    <t>OKAY|1034</t>
+  </si>
+  <si>
+    <t>GOOD|0.20829999999999999</t>
+  </si>
+  <si>
+    <t>OKAY|0.0706</t>
+  </si>
+  <si>
+    <t>BAD|0.0981</t>
+  </si>
+  <si>
+    <t>GOOD|0.51</t>
+  </si>
+  <si>
+    <t>BAD|46800</t>
+  </si>
+  <si>
+    <t>BAD|8.16</t>
+  </si>
+  <si>
+    <t>BAD|68</t>
+  </si>
+  <si>
+    <t>BAD|2.6839</t>
+  </si>
+  <si>
+    <t>BAD|-0.218</t>
+  </si>
+  <si>
+    <t>GOOD|0.0609</t>
+  </si>
+  <si>
+    <t>GOOD|0.0051</t>
+  </si>
+  <si>
+    <t>OKAY|-0.122</t>
+  </si>
+  <si>
+    <t>BEST|24.59</t>
+  </si>
+  <si>
+    <t>BAD|432</t>
+  </si>
+  <si>
+    <t>OKAY|21.6</t>
+  </si>
+  <si>
+    <t>BAD|0.2967</t>
+  </si>
+  <si>
+    <t>OKAY|0.0433</t>
+  </si>
+  <si>
+    <t>GOOD|0.0467</t>
+  </si>
+  <si>
+    <t>OKAY|0.46</t>
+  </si>
+  <si>
+    <t>OKAY|38</t>
+  </si>
+  <si>
+    <t>GOOD|-9.545346346108063</t>
+  </si>
+  <si>
+    <t>BAD|595</t>
+  </si>
+  <si>
+    <t>BAD|150</t>
+  </si>
+  <si>
+    <t>GOOD|3.966666666666667</t>
+  </si>
+  <si>
+    <t>BAD|0.5902000000000001</t>
+  </si>
+  <si>
+    <t>GOOD|-0.1411</t>
+  </si>
+  <si>
+    <t>OKAY|0.0156</t>
+  </si>
+  <si>
+    <t>BEST|-0.0458</t>
+  </si>
+  <si>
+    <t>OKAY|-0.172</t>
+  </si>
+  <si>
+    <t>BAD|50040</t>
+  </si>
+  <si>
+    <t>BAD|390</t>
+  </si>
+  <si>
+    <t>OKAY|153</t>
+  </si>
+  <si>
+    <t>OKAY|0.4404</t>
+  </si>
+  <si>
+    <t>GOOD|-0.0043</t>
+  </si>
+  <si>
+    <t>OKAY|0.0005</t>
+  </si>
+  <si>
+    <t>OKAY|-0.0267</t>
+  </si>
+  <si>
+    <t>OKAY|0.04</t>
   </si>
 </sst>
 </file>
@@ -1403,8 +1469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C01A41AF-5C41-43F4-ABA6-E54911303FD1}">
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1419,7 +1485,7 @@
     <col min="10" max="10" width="26.140625" customWidth="1"/>
     <col min="11" max="12" width="15.140625" customWidth="1"/>
     <col min="13" max="13" width="27.140625" customWidth="1"/>
-    <col min="14" max="14" width="17.140625" customWidth="1"/>
+    <col min="14" max="14" width="28.5703125" customWidth="1"/>
     <col min="15" max="15" width="17" customWidth="1"/>
     <col min="16" max="16" width="16.7109375" customWidth="1"/>
     <col min="17" max="17" width="14.7109375" customWidth="1"/>
@@ -1504,52 +1570,52 @@
         <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>46</v>
+        <v>151</v>
       </c>
       <c r="F2" s="2">
         <v>1633672800</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="L2" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="N2" s="2" t="s">
-        <v>53</v>
+        <v>154</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>54</v>
+        <v>155</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>55</v>
+        <v>156</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>56</v>
+        <v>157</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>57</v>
+        <v>158</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>58</v>
+        <v>159</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>59</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -1566,57 +1632,57 @@
         <v>22</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>60</v>
+        <v>161</v>
       </c>
       <c r="F3" s="2">
         <v>1634277600</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>63</v>
+        <v>163</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="S3" s="2" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>72</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>21</v>
@@ -1628,57 +1694,57 @@
         <v>22</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>73</v>
+        <v>171</v>
       </c>
       <c r="F4" s="2">
         <v>1632463200</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>76</v>
+        <v>172</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>79</v>
+        <v>173</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>53</v>
+        <v>174</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>82</v>
+        <v>175</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>83</v>
+        <v>176</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>84</v>
+        <v>177</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>85</v>
+        <v>178</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>86</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>24</v>
@@ -1690,57 +1756,57 @@
         <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>87</v>
+        <v>180</v>
       </c>
       <c r="F5" s="2">
         <v>1634277600</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="J5" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>90</v>
+        <v>182</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>91</v>
+        <v>183</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>92</v>
+        <v>184</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>53</v>
+        <v>185</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>93</v>
+        <v>62</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>94</v>
+        <v>186</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>95</v>
+        <v>187</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>96</v>
+        <v>188</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>98</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>24</v>
@@ -1752,57 +1818,57 @@
         <v>22</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>99</v>
+        <v>190</v>
       </c>
       <c r="F6" s="2">
         <v>1633672800</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>101</v>
+        <v>191</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>102</v>
+        <v>192</v>
       </c>
       <c r="L6" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="O6" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="M6" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="P6" s="2" t="s">
-        <v>105</v>
+        <v>195</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>106</v>
+        <v>196</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>107</v>
+        <v>197</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>108</v>
+        <v>66</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>109</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>21</v>
@@ -1814,57 +1880,57 @@
         <v>22</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>110</v>
+        <v>199</v>
       </c>
       <c r="F7" s="2">
         <v>1632463200</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>112</v>
+        <v>200</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>113</v>
+        <v>201</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>114</v>
+        <v>202</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>115</v>
+        <v>203</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>116</v>
+        <v>204</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>53</v>
+        <v>205</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>117</v>
+        <v>206</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>119</v>
+        <v>207</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>120</v>
+        <v>208</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>121</v>
+        <v>209</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>122</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>24</v>
@@ -1876,57 +1942,57 @@
         <v>22</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>123</v>
+        <v>211</v>
       </c>
       <c r="F8" s="2">
         <v>1631858400</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>124</v>
+        <v>69</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>125</v>
+        <v>212</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>126</v>
+        <v>213</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>127</v>
+        <v>214</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>128</v>
+        <v>70</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>129</v>
+        <v>215</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>53</v>
+        <v>216</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>130</v>
+        <v>217</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>131</v>
+        <v>218</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>132</v>
+        <v>219</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>133</v>
+        <v>71</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>134</v>
+        <v>220</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>135</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>24</v>
@@ -1938,57 +2004,57 @@
         <v>22</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>136</v>
+        <v>222</v>
       </c>
       <c r="F9" s="2">
         <v>1634882400</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>137</v>
+        <v>223</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>138</v>
+        <v>224</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>139</v>
+        <v>225</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>140</v>
+        <v>226</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>25</v>
+        <v>153</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>141</v>
+        <v>226</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>53</v>
+        <v>227</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>142</v>
+        <v>72</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>143</v>
+        <v>73</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>144</v>
+        <v>228</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>145</v>
+        <v>74</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>146</v>
+        <v>229</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>147</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>21</v>
@@ -2000,57 +2066,57 @@
         <v>22</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>148</v>
+        <v>231</v>
       </c>
       <c r="F10" s="2">
         <v>1637305200</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>149</v>
+        <v>75</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>150</v>
+        <v>232</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>151</v>
+        <v>76</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>152</v>
+        <v>233</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>153</v>
+        <v>234</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>65</v>
+        <v>165</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>154</v>
+        <v>77</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>53</v>
+        <v>235</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>155</v>
+        <v>236</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>156</v>
+        <v>237</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>157</v>
+        <v>238</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>158</v>
+        <v>239</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>159</v>
+        <v>240</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>160</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>24</v>
@@ -2062,57 +2128,57 @@
         <v>22</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="F11" s="2">
         <v>1634277600</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>163</v>
+        <v>78</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>164</v>
+        <v>79</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>165</v>
+        <v>80</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>166</v>
+        <v>244</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>53</v>
+        <v>245</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>167</v>
+        <v>246</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>168</v>
+        <v>247</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>169</v>
+        <v>81</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>170</v>
+        <v>248</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>171</v>
+        <v>249</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>172</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>24</v>
@@ -2124,57 +2190,57 @@
         <v>22</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>173</v>
+        <v>251</v>
       </c>
       <c r="F12" s="2">
         <v>1634882400</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>137</v>
+        <v>223</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>174</v>
+        <v>252</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>175</v>
+        <v>82</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>176</v>
+        <v>253</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>177</v>
+        <v>254</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>178</v>
+        <v>255</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>53</v>
+        <v>256</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>179</v>
+        <v>257</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>180</v>
+        <v>258</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>181</v>
+        <v>259</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>182</v>
+        <v>260</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>183</v>
+        <v>83</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>184</v>
+        <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>21</v>
@@ -2186,57 +2252,57 @@
         <v>22</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>185</v>
+        <v>262</v>
       </c>
       <c r="F13" s="2">
         <v>1631858400</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>124</v>
+        <v>69</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>186</v>
+        <v>84</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>187</v>
+        <v>85</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>188</v>
+        <v>263</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>189</v>
+        <v>264</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>190</v>
+        <v>86</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>53</v>
+        <v>265</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>191</v>
+        <v>87</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>192</v>
+        <v>266</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>193</v>
+        <v>267</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>194</v>
+        <v>88</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>195</v>
+        <v>89</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>109</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>24</v>
@@ -2248,57 +2314,57 @@
         <v>22</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>196</v>
+        <v>268</v>
       </c>
       <c r="F14" s="2">
         <v>1633068000</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>197</v>
+        <v>269</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>198</v>
+        <v>90</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>199</v>
+        <v>91</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>200</v>
+        <v>270</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>201</v>
+        <v>92</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>202</v>
+        <v>271</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>53</v>
+        <v>272</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>203</v>
+        <v>93</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>204</v>
+        <v>273</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>205</v>
+        <v>274</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>206</v>
+        <v>94</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>207</v>
+        <v>95</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>208</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>24</v>
@@ -2310,57 +2376,57 @@
         <v>22</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>209</v>
+        <v>97</v>
       </c>
       <c r="F15" s="2">
         <v>1634277600</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>210</v>
+        <v>275</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>211</v>
+        <v>98</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>212</v>
+        <v>99</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>213</v>
+        <v>100</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>214</v>
+        <v>276</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>53</v>
+        <v>277</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>215</v>
+        <v>278</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>216</v>
+        <v>279</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>217</v>
+        <v>280</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>218</v>
+        <v>281</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>219</v>
+        <v>101</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>220</v>
+        <v>282</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>24</v>
@@ -2372,57 +2438,57 @@
         <v>22</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>221</v>
+        <v>283</v>
       </c>
       <c r="F16" s="2">
         <v>1634277600</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>222</v>
+        <v>284</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>223</v>
+        <v>285</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>224</v>
+        <v>286</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>225</v>
+        <v>287</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>226</v>
+        <v>288</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>227</v>
+        <v>102</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>53</v>
+        <v>289</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>228</v>
+        <v>103</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>229</v>
+        <v>104</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>230</v>
+        <v>290</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>231</v>
+        <v>291</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>232</v>
+        <v>105</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>233</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>24</v>
@@ -2434,57 +2500,57 @@
         <v>22</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>234</v>
+        <v>107</v>
       </c>
       <c r="F17" s="2">
         <v>1642748400</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>235</v>
+        <v>292</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>236</v>
+        <v>293</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>237</v>
+        <v>108</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>238</v>
+        <v>109</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>239</v>
+        <v>294</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>53</v>
+        <v>295</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>240</v>
+        <v>296</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>241</v>
+        <v>110</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>242</v>
+        <v>297</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>243</v>
+        <v>298</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>244</v>
+        <v>111</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>245</v>
+        <v>299</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>24</v>
@@ -2496,57 +2562,57 @@
         <v>22</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>246</v>
+        <v>112</v>
       </c>
       <c r="F18" s="2">
         <v>1637305200</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>149</v>
+        <v>75</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>247</v>
+        <v>113</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>248</v>
+        <v>114</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>249</v>
+        <v>300</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>250</v>
+        <v>115</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>251</v>
+        <v>116</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>53</v>
+        <v>301</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>252</v>
+        <v>302</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>253</v>
+        <v>117</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>254</v>
+        <v>118</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>255</v>
+        <v>303</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>256</v>
+        <v>304</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>257</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>24</v>
@@ -2558,57 +2624,57 @@
         <v>22</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>258</v>
+        <v>305</v>
       </c>
       <c r="F19" s="2">
         <v>1631253600</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>259</v>
+        <v>306</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>260</v>
+        <v>120</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>261</v>
+        <v>307</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>262</v>
+        <v>308</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>263</v>
+        <v>121</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>264</v>
+        <v>122</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>53</v>
+        <v>309</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>265</v>
+        <v>310</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>266</v>
+        <v>311</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>267</v>
+        <v>312</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>268</v>
+        <v>313</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>269</v>
+        <v>314</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>270</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>24</v>
@@ -2620,57 +2686,57 @@
         <v>22</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>271</v>
+        <v>315</v>
       </c>
       <c r="F20" s="2">
         <v>1634882400</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>137</v>
+        <v>223</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>272</v>
+        <v>316</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>273</v>
+        <v>124</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>25</v>
+        <v>153</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>275</v>
+        <v>125</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>53</v>
+        <v>318</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>276</v>
+        <v>319</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>277</v>
+        <v>126</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>278</v>
+        <v>320</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>279</v>
+        <v>127</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>280</v>
+        <v>128</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>281</v>
+        <v>321</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>21</v>
@@ -2682,57 +2748,57 @@
         <v>22</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>282</v>
+        <v>322</v>
       </c>
       <c r="F21" s="2">
         <v>1632463200</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>283</v>
+        <v>129</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>284</v>
+        <v>323</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>285</v>
+        <v>130</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>286</v>
+        <v>131</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>287</v>
+        <v>324</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>288</v>
+        <v>132</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>53</v>
+        <v>325</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>289</v>
+        <v>326</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>290</v>
+        <v>327</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>291</v>
+        <v>328</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>292</v>
+        <v>133</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>293</v>
+        <v>329</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>109</v>
+        <v>198</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>24</v>
@@ -2744,57 +2810,57 @@
         <v>22</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>294</v>
+        <v>134</v>
       </c>
       <c r="F22" s="2">
         <v>1649916000</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>295</v>
+        <v>135</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>296</v>
+        <v>136</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>297</v>
+        <v>330</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>298</v>
+        <v>331</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>91</v>
+        <v>183</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>299</v>
+        <v>332</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>53</v>
+        <v>333</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>300</v>
+        <v>137</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>301</v>
+        <v>334</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>302</v>
+        <v>335</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>303</v>
+        <v>138</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>304</v>
+        <v>139</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>305</v>
+        <v>336</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>21</v>
@@ -2806,57 +2872,57 @@
         <v>22</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>306</v>
+        <v>140</v>
       </c>
       <c r="F23" s="2">
         <v>1631858400</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>124</v>
+        <v>69</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>307</v>
+        <v>337</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>308</v>
+        <v>141</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>309</v>
+        <v>338</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>310</v>
+        <v>339</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>311</v>
+        <v>340</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>312</v>
+        <v>341</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>53</v>
+        <v>342</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>313</v>
+        <v>343</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>314</v>
+        <v>142</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>315</v>
+        <v>344</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>316</v>
+        <v>345</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>317</v>
+        <v>346</v>
       </c>
       <c r="T23" s="2" t="s">
-        <v>318</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>21</v>
@@ -2868,52 +2934,52 @@
         <v>22</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>319</v>
+        <v>347</v>
       </c>
       <c r="F24" s="2">
         <v>1631512800</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>320</v>
+        <v>144</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>321</v>
+        <v>348</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>322</v>
+        <v>145</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>323</v>
+        <v>146</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>324</v>
+        <v>147</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>325</v>
+        <v>349</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>326</v>
+        <v>148</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>53</v>
+        <v>350</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>327</v>
+        <v>351</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>328</v>
+        <v>352</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>329</v>
+        <v>149</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>330</v>
+        <v>353</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>331</v>
+        <v>150</v>
       </c>
       <c r="T24" s="2" t="s">
-        <v>332</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix realtime diff calculation
</commit_message>
<xml_diff>
--- a/data/options-recap/realtime/excel/Options Recap.xlsx
+++ b/data/options-recap/realtime/excel/Options Recap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Programming\Cue\data\options-recap\realtime\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08B1285-62AB-449D-B320-1D235BD4B742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13903EA-1DE7-4925-9D2A-32D297420C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{46699434-473C-4966-BCFA-04206E4C53EA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="368">
   <si>
     <t>Ticker</t>
   </si>
@@ -186,9 +186,6 @@
     <t>GOOD|6001</t>
   </si>
   <si>
-    <t>|0</t>
-  </si>
-  <si>
     <t>OKAY|12.5</t>
   </si>
   <si>
@@ -291,9 +288,6 @@
     <t>OKAY|7.09</t>
   </si>
   <si>
-    <t>GOOD|41.000000000000014</t>
-  </si>
-  <si>
     <t>BAD|7.684085510688836</t>
   </si>
   <si>
@@ -894,9 +888,6 @@
     <t>BEST|5.05</t>
   </si>
   <si>
-    <t>OKAY|45.000000000000014</t>
-  </si>
-  <si>
     <t>OKAY|3115</t>
   </si>
   <si>
@@ -1099,6 +1090,54 @@
   </si>
   <si>
     <t>OKAY|0.04</t>
+  </si>
+  <si>
+    <t>BAD|25.125125125125123</t>
+  </si>
+  <si>
+    <t>OKAY|5.42377583576085</t>
+  </si>
+  <si>
+    <t>BEST|5.762217359591532</t>
+  </si>
+  <si>
+    <t>BEST|5.0769870994590045</t>
+  </si>
+  <si>
+    <t>BAD|28.39030653185684</t>
+  </si>
+  <si>
+    <t>BAD|17.004680187207484</t>
+  </si>
+  <si>
+    <t>GOOD|10.803324099722996</t>
+  </si>
+  <si>
+    <t>OKAY|5.782792665726378</t>
+  </si>
+  <si>
+    <t>BAD|6.052294752239902</t>
+  </si>
+  <si>
+    <t>BAD|12.8233351678591</t>
+  </si>
+  <si>
+    <t>BAD|8.910891089108915</t>
+  </si>
+  <si>
+    <t>BAD|35.13513513513514</t>
+  </si>
+  <si>
+    <t>GOOD|24.89592006661117</t>
+  </si>
+  <si>
+    <t>OKAY|5.345911949685532</t>
+  </si>
+  <si>
+    <t>BEST|11.417914062878454</t>
+  </si>
+  <si>
+    <t>BAD|26.06750711671411</t>
   </si>
 </sst>
 </file>
@@ -1470,7 +1509,7 @@
   <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1570,7 +1609,7 @@
         <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F2" s="2">
         <v>1633672800</v>
@@ -1579,7 +1618,7 @@
         <v>45</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>46</v>
@@ -1591,31 +1630,31 @@
         <v>48</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>49</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -1632,52 +1671,52 @@
         <v>22</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F3" s="2">
         <v>1634277600</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="L3" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="P3" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="P3" s="2" t="s">
+      <c r="S3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="T3" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -1694,52 +1733,52 @@
         <v>22</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F4" s="2">
         <v>1632463200</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="K4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="L4" s="2" t="s">
+      <c r="O4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="M4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="N4" s="2" t="s">
+      <c r="Q4" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="O4" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="P4" s="2" t="s">
+      <c r="R4" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="S4" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="T4" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -1756,52 +1795,52 @@
         <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F5" s="2">
         <v>1634277600</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H5" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="M5" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="O5" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="M5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="Q5" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="R5" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="S5" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="P5" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="Q5" s="2" t="s">
+      <c r="T5" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -1818,7 +1857,7 @@
         <v>22</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F6" s="2">
         <v>1633672800</v>
@@ -1827,43 +1866,43 @@
         <v>45</v>
       </c>
       <c r="H6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="O6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="M6" s="2" t="s">
+      <c r="P6" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="Q6" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="R6" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="S6" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P6" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q6" s="2" t="s">
+      <c r="T6" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="T6" s="2" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -1880,52 +1919,52 @@
         <v>22</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F7" s="2">
         <v>1632463200</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="P7" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="N7" s="2" t="s">
+      <c r="Q7" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="R7" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="P7" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q7" s="2" t="s">
+      <c r="S7" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="R7" s="2" t="s">
+      <c r="T7" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="T7" s="2" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -1942,52 +1981,52 @@
         <v>22</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F8" s="2">
         <v>1631858400</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="I8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K8" s="2" t="s">
+      <c r="N8" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="O8" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="R8" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="M8" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="P8" s="2" t="s">
+      <c r="S8" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="T8" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="S8" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="T8" s="2" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -2004,52 +2043,52 @@
         <v>22</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F9" s="2">
         <v>1634882400</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="J9" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="L9" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="N9" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K9" s="2" t="s">
+      <c r="O9" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q9" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="L9" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="N9" s="2" t="s">
+      <c r="R9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="S9" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="O9" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q9" s="2" t="s">
+      <c r="T9" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="R9" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="S9" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="T9" s="2" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -2066,52 +2105,52 @@
         <v>22</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F10" s="2">
         <v>1637305200</v>
       </c>
       <c r="G10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="J10" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="L10" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="M10" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="N10" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="O10" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="L10" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="N10" s="2" t="s">
+      <c r="P10" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="Q10" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="P10" s="2" t="s">
+      <c r="R10" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="Q10" s="2" t="s">
+      <c r="S10" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="R10" s="2" t="s">
+      <c r="T10" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="S10" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="T10" s="2" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -2128,52 +2167,52 @@
         <v>22</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F11" s="2">
         <v>1634277600</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H11" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="N11" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="L11" s="2" t="s">
+      <c r="O11" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q11" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="M11" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="O11" s="2" t="s">
+      <c r="R11" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="P11" s="2" t="s">
+      <c r="S11" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="Q11" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="R11" s="2" t="s">
+      <c r="T11" s="2" t="s">
         <v>248</v>
-      </c>
-      <c r="S11" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="T11" s="2" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -2190,52 +2229,52 @@
         <v>22</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F12" s="2">
         <v>1634882400</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H12" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="M12" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="S12" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="J12" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="Q12" s="2" t="s">
+      <c r="T12" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="S12" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="T12" s="2" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -2252,52 +2291,52 @@
         <v>22</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F13" s="2">
         <v>1631858400</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="I13" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="M13" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="N13" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="O13" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="K13" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="L13" s="2" t="s">
+      <c r="P13" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="Q13" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="R13" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="N13" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="O13" s="2" t="s">
+      <c r="S13" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="P13" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="R13" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="S13" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="T13" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -2314,52 +2353,52 @@
         <v>22</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F14" s="2">
         <v>1633068000</v>
       </c>
       <c r="G14" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M14" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="I14" s="2" t="s">
+      <c r="N14" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="O14" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="L14" s="2" t="s">
+      <c r="P14" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="R14" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="M14" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="O14" s="2" t="s">
+      <c r="S14" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="P14" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="Q14" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="R14" s="2" t="s">
+      <c r="T14" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="S14" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="T14" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -2376,52 +2415,52 @@
         <v>22</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F15" s="2">
         <v>1634277600</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H15" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="N15" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K15" s="2" t="s">
+      <c r="O15" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="S15" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L15" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="Q15" s="2" t="s">
+      <c r="T15" s="2" t="s">
         <v>280</v>
-      </c>
-      <c r="R15" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="S15" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="T15" s="2" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -2438,52 +2477,52 @@
         <v>22</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F16" s="2">
         <v>1634277600</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H16" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="K16" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="L16" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="M16" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N16" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="O16" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q16" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="R16" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="M16" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="O16" s="2" t="s">
+      <c r="S16" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="P16" s="2" t="s">
+      <c r="T16" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="Q16" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="R16" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="S16" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="T16" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
@@ -2500,52 +2539,52 @@
         <v>22</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F17" s="2">
         <v>1642748400</v>
       </c>
       <c r="G17" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="N17" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I17" s="2" t="s">
+      <c r="O17" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="J17" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K17" s="2" t="s">
+      <c r="P17" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="Q17" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="S17" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="M17" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="N17" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="O17" s="2" t="s">
+      <c r="T17" s="2" t="s">
         <v>296</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q17" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="R17" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="S17" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="T17" s="2" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
@@ -2562,52 +2601,52 @@
         <v>22</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F18" s="2">
         <v>1637305200</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H18" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="L18" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="M18" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="J18" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K18" s="2" t="s">
+      <c r="N18" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="R18" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="L18" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="N18" s="2" t="s">
+      <c r="S18" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="O18" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="P18" s="2" t="s">
+      <c r="T18" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="Q18" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="R18" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="S18" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="T18" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
@@ -2624,52 +2663,52 @@
         <v>22</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="F19" s="2">
         <v>1631253600</v>
       </c>
       <c r="G19" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="N19" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="I19" s="2" t="s">
+      <c r="O19" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="J19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K19" s="2" t="s">
+      <c r="P19" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="L19" s="2" t="s">
+      <c r="Q19" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="S19" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="T19" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="N19" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="O19" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="P19" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="Q19" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="R19" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="S19" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="T19" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
@@ -2686,52 +2725,52 @@
         <v>22</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="F20" s="2">
         <v>1634882400</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H20" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="O20" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="P20" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="J20" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K20" s="2" t="s">
+      <c r="Q20" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="L20" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="M20" s="2" t="s">
+      <c r="R20" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="N20" s="2" t="s">
+      <c r="S20" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="T20" s="2" t="s">
         <v>318</v>
-      </c>
-      <c r="O20" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q20" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="R20" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="S20" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="T20" s="2" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
@@ -2748,52 +2787,52 @@
         <v>22</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="F21" s="2">
         <v>1632463200</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H21" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="K21" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="L21" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="O21" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="J21" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="K21" s="2" t="s">
+      <c r="P21" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="R21" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="L21" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="N21" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="O21" s="2" t="s">
+      <c r="S21" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="P21" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="Q21" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="R21" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="S21" s="2" t="s">
-        <v>329</v>
-      </c>
       <c r="T21" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
@@ -2810,52 +2849,52 @@
         <v>22</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F22" s="2">
         <v>1649916000</v>
       </c>
       <c r="G22" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="O22" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="P22" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="R22" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="I22" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="N22" s="2" t="s">
+      <c r="S22" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="T22" s="2" t="s">
         <v>333</v>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="P22" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="Q22" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="R22" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="S22" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="T22" s="2" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
@@ -2872,52 +2911,52 @@
         <v>22</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F23" s="2">
         <v>1631858400</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H23" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="L23" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="M23" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="S23" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="T23" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="N23" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="O23" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="P23" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q23" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="R23" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="S23" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="T23" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
@@ -2934,52 +2973,52 @@
         <v>22</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="F24" s="2">
         <v>1631512800</v>
       </c>
       <c r="G24" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="J24" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="K24" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="O24" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="I24" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="K24" s="2" t="s">
+      <c r="P24" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="Q24" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="L24" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="M24" s="2" t="s">
+      <c r="R24" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="S24" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="N24" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="O24" s="2" t="s">
+      <c r="T24" s="2" t="s">
         <v>351</v>
-      </c>
-      <c r="P24" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="Q24" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="R24" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="S24" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="T24" s="2" t="s">
-        <v>354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Seperate call and put rating logic
</commit_message>
<xml_diff>
--- a/data/options-recap/realtime/excel/Options Recap.xlsx
+++ b/data/options-recap/realtime/excel/Options Recap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Programming\Cue\data\options-recap\realtime\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13903EA-1DE7-4925-9D2A-32D297420C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E04CEACB-69EB-477E-864D-2A48DC4A2939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{46699434-473C-4966-BCFA-04206E4C53EA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="372">
   <si>
     <t>Ticker</t>
   </si>
@@ -186,12 +186,6 @@
     <t>GOOD|6001</t>
   </si>
   <si>
-    <t>OKAY|12.5</t>
-  </si>
-  <si>
-    <t>OKAY|744.6666666666666</t>
-  </si>
-  <si>
     <t>BAD|-0.0049</t>
   </si>
   <si>
@@ -207,18 +201,12 @@
     <t>BAD|-5.412506568575937</t>
   </si>
   <si>
-    <t>BAD|12449</t>
-  </si>
-  <si>
     <t>BAD|57.63425925925926</t>
   </si>
   <si>
     <t>BAD|-0.1576</t>
   </si>
   <si>
-    <t>OKAY|72.09</t>
-  </si>
-  <si>
     <t>GOOD|0.1643</t>
   </si>
   <si>
@@ -237,9 +225,6 @@
     <t>OKAY|104.5</t>
   </si>
   <si>
-    <t>OKAY|0.0473</t>
-  </si>
-  <si>
     <t>OKAY|9</t>
   </si>
   <si>
@@ -255,39 +240,21 @@
     <t>OKAY|0.0158</t>
   </si>
   <si>
-    <t>OKAY|-0.0238</t>
-  </si>
-  <si>
     <t>GOOD|72</t>
   </si>
   <si>
     <t>OKAY|36.48</t>
   </si>
   <si>
-    <t>BEST|194</t>
-  </si>
-  <si>
-    <t>GOOD|6.41</t>
-  </si>
-  <si>
-    <t>BAD|6722</t>
-  </si>
-  <si>
     <t>BAD|822</t>
   </si>
   <si>
     <t>OKAY|0.0079</t>
   </si>
   <si>
-    <t>BAD|7.22</t>
-  </si>
-  <si>
     <t>BAD|0.2804</t>
   </si>
   <si>
-    <t>OKAY|7.09</t>
-  </si>
-  <si>
     <t>BAD|7.684085510688836</t>
   </si>
   <si>
@@ -300,12 +267,6 @@
     <t>OKAY|-0.1383</t>
   </si>
   <si>
-    <t>OKAY|58</t>
-  </si>
-  <si>
-    <t>GOOD|54.69</t>
-  </si>
-  <si>
     <t>OKAY|587</t>
   </si>
   <si>
@@ -318,21 +279,12 @@
     <t>BAD|0.687</t>
   </si>
   <si>
-    <t>OKAY|0.39</t>
-  </si>
-  <si>
     <t>BAD|40620</t>
   </si>
   <si>
     <t>OKAY|36.34</t>
   </si>
   <si>
-    <t>BAD|6107</t>
-  </si>
-  <si>
-    <t>BAD|1789</t>
-  </si>
-  <si>
     <t>BAD|0.4122</t>
   </si>
   <si>
@@ -351,9 +303,6 @@
     <t>OKAY|0.23</t>
   </si>
   <si>
-    <t>GOOD|43020</t>
-  </si>
-  <si>
     <t>BAD|15035</t>
   </si>
   <si>
@@ -369,21 +318,9 @@
     <t>BAD|43200</t>
   </si>
   <si>
-    <t>OKAY|105</t>
-  </si>
-  <si>
-    <t>BAD|84.07</t>
-  </si>
-  <si>
-    <t>BAD|24</t>
-  </si>
-  <si>
     <t>OKAY|23.5</t>
   </si>
   <si>
-    <t>OKAY|0.0131</t>
-  </si>
-  <si>
     <t>OKAY|0.0727</t>
   </si>
   <si>
@@ -408,9 +345,6 @@
     <t>BAD|1034</t>
   </si>
   <si>
-    <t>OKAY|0.0089</t>
-  </si>
-  <si>
     <t>OKAY|-0.022</t>
   </si>
   <si>
@@ -423,21 +357,12 @@
     <t>BAD|-26.470588235294123</t>
   </si>
   <si>
-    <t>GOOD|442</t>
-  </si>
-  <si>
-    <t>BAD|6.5</t>
-  </si>
-  <si>
     <t>OKAY|-0.0448</t>
   </si>
   <si>
     <t>BAD|47340</t>
   </si>
   <si>
-    <t>OKAY|218</t>
-  </si>
-  <si>
     <t>BAD|31</t>
   </si>
   <si>
@@ -450,15 +375,9 @@
     <t>OKAY|2.1443</t>
   </si>
   <si>
-    <t>BAD|47820</t>
-  </si>
-  <si>
     <t>BAD|42.01</t>
   </si>
   <si>
-    <t>OKAY|0.0543</t>
-  </si>
-  <si>
     <t>GOOD|0.32</t>
   </si>
   <si>
@@ -474,18 +393,9 @@
     <t>BAD|11521</t>
   </si>
   <si>
-    <t>BAD|75.30065359477125</t>
-  </si>
-  <si>
-    <t>BEST|0.0073</t>
-  </si>
-  <si>
     <t>BAD|-0.0325</t>
   </si>
   <si>
-    <t>BAD|30420</t>
-  </si>
-  <si>
     <t>GOOD|39.5</t>
   </si>
   <si>
@@ -501,9 +411,6 @@
     <t>BEST|0.0751</t>
   </si>
   <si>
-    <t>GOOD|0.0339</t>
-  </si>
-  <si>
     <t>GOOD|-0.0158</t>
   </si>
   <si>
@@ -558,12 +465,6 @@
     <t>OKAY|0.1167</t>
   </si>
   <si>
-    <t>BEST|0.0199</t>
-  </si>
-  <si>
-    <t>BEST|-0.0153</t>
-  </si>
-  <si>
     <t>BEST|-0.2918</t>
   </si>
   <si>
@@ -573,27 +474,18 @@
     <t>OKAY|32580</t>
   </si>
   <si>
-    <t>BAD|76</t>
-  </si>
-  <si>
     <t>BAD|4625</t>
   </si>
   <si>
     <t>BAD|20</t>
   </si>
   <si>
-    <t>OKAY|231.25</t>
-  </si>
-  <si>
     <t>BAD|0.1648</t>
   </si>
   <si>
     <t>BAD|0.0644</t>
   </si>
   <si>
-    <t>OKAY|0.0577</t>
-  </si>
-  <si>
     <t>OKAY|-0.0124</t>
   </si>
   <si>
@@ -603,9 +495,6 @@
     <t>BAD|32700</t>
   </si>
   <si>
-    <t>OKAY|13.71</t>
-  </si>
-  <si>
     <t>BAD|400</t>
   </si>
   <si>
@@ -615,9 +504,6 @@
     <t>GOOD|0.7059000000000001</t>
   </si>
   <si>
-    <t>OKAY|0.1383</t>
-  </si>
-  <si>
     <t>BAD|0.0159</t>
   </si>
   <si>
@@ -645,9 +531,6 @@
     <t>BAD|255</t>
   </si>
   <si>
-    <t>BAD|0.21170000000000003</t>
-  </si>
-  <si>
     <t>BEST|-0.1557</t>
   </si>
   <si>
@@ -663,24 +546,9 @@
     <t>OKAY|0.44</t>
   </si>
   <si>
-    <t>BEST|34440</t>
-  </si>
-  <si>
     <t>OKAY|50.5</t>
   </si>
   <si>
-    <t>OKAY|48.06</t>
-  </si>
-  <si>
-    <t>OKAY|3074</t>
-  </si>
-  <si>
-    <t>BEST|6.682608695652174</t>
-  </si>
-  <si>
-    <t>OKAY|0.33630000000000004</t>
-  </si>
-  <si>
     <t>BAD|0.1976</t>
   </si>
   <si>
@@ -699,24 +567,12 @@
     <t>OKAY|34980</t>
   </si>
   <si>
-    <t>GOOD|44</t>
-  </si>
-  <si>
-    <t>OKAY|80</t>
-  </si>
-  <si>
-    <t>GOOD|62.31</t>
-  </si>
-  <si>
     <t>GOOD|263</t>
   </si>
   <si>
     <t>BAD|0.5324</t>
   </si>
   <si>
-    <t>OKAY|0.0404</t>
-  </si>
-  <si>
     <t>BAD|0.756</t>
   </si>
   <si>
@@ -726,9 +582,6 @@
     <t>BAD|35640</t>
   </si>
   <si>
-    <t>BAD|32</t>
-  </si>
-  <si>
     <t>BAD|-12.280701754385959</t>
   </si>
   <si>
@@ -747,18 +600,9 @@
     <t>BEST|0.0457</t>
   </si>
   <si>
-    <t>GOOD|-0.0121</t>
-  </si>
-  <si>
     <t>BAD|-1.6171</t>
   </si>
   <si>
-    <t>GOOD|0.78</t>
-  </si>
-  <si>
-    <t>GOOD|35880</t>
-  </si>
-  <si>
     <t>OKAY|7.5</t>
   </si>
   <si>
@@ -807,9 +651,6 @@
     <t>GOOD|0.2258</t>
   </si>
   <si>
-    <t>GOOD|0.0095</t>
-  </si>
-  <si>
     <t>OKAY|-0.0067</t>
   </si>
   <si>
@@ -822,9 +663,6 @@
     <t>BAD|3235</t>
   </si>
   <si>
-    <t>OKAY|421</t>
-  </si>
-  <si>
     <t>OKAY|1.2604</t>
   </si>
   <si>
@@ -834,18 +672,9 @@
     <t>BAD|0.0046</t>
   </si>
   <si>
-    <t>BEST|40080</t>
-  </si>
-  <si>
-    <t>OKAY|23</t>
-  </si>
-  <si>
     <t>GOOD|3735</t>
   </si>
   <si>
-    <t>OKAY|6.362862010221465</t>
-  </si>
-  <si>
     <t>OKAY|0.258</t>
   </si>
   <si>
@@ -858,12 +687,6 @@
     <t>OKAY|41</t>
   </si>
   <si>
-    <t>BAD|3.413638904415875</t>
-  </si>
-  <si>
-    <t>OKAY|0.2961</t>
-  </si>
-  <si>
     <t>BAD|0.1135</t>
   </si>
   <si>
@@ -876,39 +699,24 @@
     <t>OKAY|-0.0088</t>
   </si>
   <si>
-    <t>GOOD|0.19</t>
-  </si>
-  <si>
-    <t>OKAY|42120</t>
-  </si>
-  <si>
     <t>OKAY|5.5</t>
   </si>
   <si>
     <t>BEST|5.05</t>
   </si>
   <si>
-    <t>OKAY|3115</t>
-  </si>
-  <si>
     <t>BAD|569</t>
   </si>
   <si>
     <t>BAD|0.5981000000000001</t>
   </si>
   <si>
-    <t>BAD|0.0061</t>
-  </si>
-  <si>
     <t>OKAY|-0.0047</t>
   </si>
   <si>
     <t>GOOD|135</t>
   </si>
   <si>
-    <t>BAD|9.25</t>
-  </si>
-  <si>
     <t>GOOD|38.452685421994886</t>
   </si>
   <si>
@@ -927,12 +735,6 @@
     <t>OKAY|0.2</t>
   </si>
   <si>
-    <t>OKAY|564</t>
-  </si>
-  <si>
-    <t>OKAY|0.39149999999999996</t>
-  </si>
-  <si>
     <t>BAD|0.1143</t>
   </si>
   <si>
@@ -942,12 +744,6 @@
     <t>GOOD|1.7741</t>
   </si>
   <si>
-    <t>OKAY|43860</t>
-  </si>
-  <si>
-    <t>GOOD|2</t>
-  </si>
-  <si>
     <t>OKAY|31.8</t>
   </si>
   <si>
@@ -972,27 +768,18 @@
     <t>GOOD|0.0845</t>
   </si>
   <si>
-    <t>GOOD|43980</t>
-  </si>
-  <si>
     <t>BEST|230</t>
   </si>
   <si>
     <t>OKAY|1034</t>
   </si>
   <si>
-    <t>GOOD|0.20829999999999999</t>
-  </si>
-  <si>
     <t>OKAY|0.0706</t>
   </si>
   <si>
     <t>BAD|0.0981</t>
   </si>
   <si>
-    <t>GOOD|0.51</t>
-  </si>
-  <si>
     <t>BAD|46800</t>
   </si>
   <si>
@@ -1011,36 +798,18 @@
     <t>GOOD|0.0609</t>
   </si>
   <si>
-    <t>GOOD|0.0051</t>
-  </si>
-  <si>
     <t>OKAY|-0.122</t>
   </si>
   <si>
-    <t>BEST|24.59</t>
-  </si>
-  <si>
     <t>BAD|432</t>
   </si>
   <si>
-    <t>OKAY|21.6</t>
-  </si>
-  <si>
     <t>BAD|0.2967</t>
   </si>
   <si>
     <t>OKAY|0.0433</t>
   </si>
   <si>
-    <t>GOOD|0.0467</t>
-  </si>
-  <si>
-    <t>OKAY|0.46</t>
-  </si>
-  <si>
-    <t>OKAY|38</t>
-  </si>
-  <si>
     <t>GOOD|-9.545346346108063</t>
   </si>
   <si>
@@ -1050,9 +819,6 @@
     <t>BAD|150</t>
   </si>
   <si>
-    <t>GOOD|3.966666666666667</t>
-  </si>
-  <si>
     <t>BAD|0.5902000000000001</t>
   </si>
   <si>
@@ -1062,9 +828,6 @@
     <t>OKAY|0.0156</t>
   </si>
   <si>
-    <t>BEST|-0.0458</t>
-  </si>
-  <si>
     <t>OKAY|-0.172</t>
   </si>
   <si>
@@ -1089,9 +852,6 @@
     <t>OKAY|-0.0267</t>
   </si>
   <si>
-    <t>OKAY|0.04</t>
-  </si>
-  <si>
     <t>BAD|25.125125125125123</t>
   </si>
   <si>
@@ -1113,9 +873,6 @@
     <t>GOOD|10.803324099722996</t>
   </si>
   <si>
-    <t>OKAY|5.782792665726378</t>
-  </si>
-  <si>
     <t>BAD|6.052294752239902</t>
   </si>
   <si>
@@ -1138,6 +895,261 @@
   </si>
   <si>
     <t>BAD|26.06750711671411</t>
+  </si>
+  <si>
+    <t>OKAY|30420</t>
+  </si>
+  <si>
+    <t>GOOD|30</t>
+  </si>
+  <si>
+    <t>OKAY|0.0339</t>
+  </si>
+  <si>
+    <t>GOOD|12.5</t>
+  </si>
+  <si>
+    <t>BAD|744.6666666666666</t>
+  </si>
+  <si>
+    <t>BEST|12449</t>
+  </si>
+  <si>
+    <t>OKAY|0.0199</t>
+  </si>
+  <si>
+    <t>OKAY|-0.0153</t>
+  </si>
+  <si>
+    <t>OKAY|76</t>
+  </si>
+  <si>
+    <t>BAD|72.09</t>
+  </si>
+  <si>
+    <t>BAD|231.25</t>
+  </si>
+  <si>
+    <t>BAD|0.0577</t>
+  </si>
+  <si>
+    <t>BAD|13.71</t>
+  </si>
+  <si>
+    <t>BAD|0.1383</t>
+  </si>
+  <si>
+    <t>GOOD|0.21170000000000003</t>
+  </si>
+  <si>
+    <t>BAD|0.0473</t>
+  </si>
+  <si>
+    <t>BAD|34440</t>
+  </si>
+  <si>
+    <t>BAD|48.06</t>
+  </si>
+  <si>
+    <t>GOOD|3074</t>
+  </si>
+  <si>
+    <t>BAD|6.682608695652174</t>
+  </si>
+  <si>
+    <t>GOOD|0.33630000000000004</t>
+  </si>
+  <si>
+    <t>BAD|44</t>
+  </si>
+  <si>
+    <t>BAD|80</t>
+  </si>
+  <si>
+    <t>OKAY|62.31</t>
+  </si>
+  <si>
+    <t>OKAY|1</t>
+  </si>
+  <si>
+    <t>BAD|0.0404</t>
+  </si>
+  <si>
+    <t>GOOD|-0.0238</t>
+  </si>
+  <si>
+    <t>BEST|32</t>
+  </si>
+  <si>
+    <t>BAD|194</t>
+  </si>
+  <si>
+    <t>OKAY|-0.0121</t>
+  </si>
+  <si>
+    <t>OKAY|0.78</t>
+  </si>
+  <si>
+    <t>BAD|35880</t>
+  </si>
+  <si>
+    <t>BEST|7.5</t>
+  </si>
+  <si>
+    <t>OKAY|6.41</t>
+  </si>
+  <si>
+    <t>OKAY|6722</t>
+  </si>
+  <si>
+    <t>BEST|7.22</t>
+  </si>
+  <si>
+    <t>OKAY|0.0095</t>
+  </si>
+  <si>
+    <t>GOOD|7.09</t>
+  </si>
+  <si>
+    <t>GOOD|5.782792665726378</t>
+  </si>
+  <si>
+    <t>BAD|421</t>
+  </si>
+  <si>
+    <t>OKAY|40080</t>
+  </si>
+  <si>
+    <t>BAD|23</t>
+  </si>
+  <si>
+    <t>GOOD|58</t>
+  </si>
+  <si>
+    <t>OKAY|54.69</t>
+  </si>
+  <si>
+    <t>BAD|6.362862010221465</t>
+  </si>
+  <si>
+    <t>GOOD|0.39</t>
+  </si>
+  <si>
+    <t>OKAY|6107</t>
+  </si>
+  <si>
+    <t>OKAY|1789</t>
+  </si>
+  <si>
+    <t>OKAY|3.413638904415875</t>
+  </si>
+  <si>
+    <t>BEST|0.2961</t>
+  </si>
+  <si>
+    <t>OKAY|0.19</t>
+  </si>
+  <si>
+    <t>BAD|42120</t>
+  </si>
+  <si>
+    <t>BAD|3115</t>
+  </si>
+  <si>
+    <t>OKAY|0.0061</t>
+  </si>
+  <si>
+    <t>BAD|43020</t>
+  </si>
+  <si>
+    <t>OKAY|9.25</t>
+  </si>
+  <si>
+    <t>BEST|72</t>
+  </si>
+  <si>
+    <t>BEST|105</t>
+  </si>
+  <si>
+    <t>OKAY|84.07</t>
+  </si>
+  <si>
+    <t>BAD|564</t>
+  </si>
+  <si>
+    <t>GOOD|24</t>
+  </si>
+  <si>
+    <t>GOOD|0.39149999999999996</t>
+  </si>
+  <si>
+    <t>BAD|0.0131</t>
+  </si>
+  <si>
+    <t>GOOD|43860</t>
+  </si>
+  <si>
+    <t>BAD|2</t>
+  </si>
+  <si>
+    <t>BAD|43980</t>
+  </si>
+  <si>
+    <t>BAD|0.20829999999999999</t>
+  </si>
+  <si>
+    <t>BAD|0.0089</t>
+  </si>
+  <si>
+    <t>BAD|0.51</t>
+  </si>
+  <si>
+    <t>BAD|442</t>
+  </si>
+  <si>
+    <t>OKAY|6.5</t>
+  </si>
+  <si>
+    <t>BAD|0.0051</t>
+  </si>
+  <si>
+    <t>BAD|218</t>
+  </si>
+  <si>
+    <t>BAD|24.59</t>
+  </si>
+  <si>
+    <t>BEST|21.6</t>
+  </si>
+  <si>
+    <t>BAD|0.0467</t>
+  </si>
+  <si>
+    <t>BAD|0.46</t>
+  </si>
+  <si>
+    <t>OKAY|47820</t>
+  </si>
+  <si>
+    <t>GOOD|38</t>
+  </si>
+  <si>
+    <t>BAD|3.966666666666667</t>
+  </si>
+  <si>
+    <t>BAD|0.0543</t>
+  </si>
+  <si>
+    <t>BAD|-0.0458</t>
+  </si>
+  <si>
+    <t>BEST|75.30065359477125</t>
+  </si>
+  <si>
+    <t>GOOD|0.0073</t>
+  </si>
+  <si>
+    <t>BAD|0.04</t>
   </si>
 </sst>
 </file>
@@ -1509,7 +1521,7 @@
   <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1609,16 +1621,16 @@
         <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>149</v>
+        <v>287</v>
       </c>
       <c r="F2" s="2">
         <v>1633672800</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>45</v>
+        <v>288</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>46</v>
@@ -1630,31 +1642,31 @@
         <v>48</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>151</v>
+        <v>121</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>49</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>152</v>
+        <v>122</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>153</v>
+        <v>123</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>154</v>
+        <v>124</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>155</v>
+        <v>289</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>157</v>
+        <v>126</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -1671,52 +1683,52 @@
         <v>22</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>159</v>
+        <v>128</v>
       </c>
       <c r="F3" s="2">
         <v>1634277600</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>160</v>
+        <v>129</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="M3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="T3" s="2" t="s">
-        <v>168</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -1733,52 +1745,52 @@
         <v>22</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>169</v>
+        <v>138</v>
       </c>
       <c r="F4" s="2">
         <v>1632463200</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="K4" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="J4" s="2" t="s">
+      <c r="N4" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="O4" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="P4" s="2" t="s">
-        <v>173</v>
+        <v>142</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>174</v>
+        <v>293</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>175</v>
+        <v>294</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>176</v>
+        <v>143</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>177</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -1795,52 +1807,52 @@
         <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>178</v>
+        <v>145</v>
       </c>
       <c r="F5" s="2">
         <v>1634277600</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>160</v>
+        <v>129</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>179</v>
+        <v>295</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>60</v>
+        <v>296</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>353</v>
+        <v>273</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>182</v>
+        <v>297</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>183</v>
+        <v>148</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>184</v>
+        <v>149</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>185</v>
+        <v>298</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>186</v>
+        <v>150</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>187</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -1857,7 +1869,7 @@
         <v>22</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>188</v>
+        <v>152</v>
       </c>
       <c r="F6" s="2">
         <v>1633672800</v>
@@ -1866,43 +1878,43 @@
         <v>45</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>189</v>
+        <v>299</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>354</v>
+        <v>274</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>190</v>
+        <v>153</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>163</v>
+        <v>132</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>191</v>
+        <v>154</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>192</v>
+        <v>155</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>193</v>
+        <v>300</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>194</v>
+        <v>156</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>195</v>
+        <v>157</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>196</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -1919,52 +1931,52 @@
         <v>22</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>197</v>
+        <v>159</v>
       </c>
       <c r="F7" s="2">
         <v>1632463200</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>198</v>
+        <v>160</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>199</v>
+        <v>161</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>200</v>
+        <v>162</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>201</v>
+        <v>163</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>202</v>
+        <v>164</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>203</v>
+        <v>301</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>204</v>
+        <v>165</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>67</v>
+        <v>302</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>205</v>
+        <v>166</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>206</v>
+        <v>167</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>207</v>
+        <v>168</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>208</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -1981,52 +1993,52 @@
         <v>22</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>209</v>
+        <v>303</v>
       </c>
       <c r="F8" s="2">
         <v>1631858400</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>210</v>
+        <v>170</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>211</v>
+        <v>304</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>355</v>
+        <v>275</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>212</v>
+        <v>305</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>213</v>
+        <v>306</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>214</v>
+        <v>307</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>215</v>
+        <v>171</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>216</v>
+        <v>172</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>217</v>
+        <v>173</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>218</v>
+        <v>174</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>219</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -2043,52 +2055,52 @@
         <v>22</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>220</v>
+        <v>176</v>
       </c>
       <c r="F9" s="2">
         <v>1634882400</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>221</v>
+        <v>308</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>222</v>
+        <v>309</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>223</v>
+        <v>310</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>356</v>
+        <v>276</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>224</v>
+        <v>177</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>151</v>
+        <v>311</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>224</v>
+        <v>177</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>225</v>
+        <v>178</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>226</v>
+        <v>312</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>73</v>
+        <v>313</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>227</v>
+        <v>179</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>228</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -2105,52 +2117,52 @@
         <v>22</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>229</v>
+        <v>181</v>
       </c>
       <c r="F10" s="2">
         <v>1637305200</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>230</v>
+        <v>314</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>231</v>
+        <v>182</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>232</v>
+        <v>183</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>163</v>
+        <v>132</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>76</v>
+        <v>315</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>233</v>
+        <v>184</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>234</v>
+        <v>185</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>235</v>
+        <v>186</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>236</v>
+        <v>187</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>237</v>
+        <v>316</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>238</v>
+        <v>188</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>239</v>
+        <v>317</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -2167,52 +2179,52 @@
         <v>22</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>240</v>
+        <v>318</v>
       </c>
       <c r="F11" s="2">
         <v>1634277600</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>160</v>
+        <v>129</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>241</v>
+        <v>319</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>77</v>
+        <v>320</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>357</v>
+        <v>277</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>78</v>
+        <v>321</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>242</v>
+        <v>190</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>243</v>
+        <v>191</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>244</v>
+        <v>192</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>245</v>
+        <v>193</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>246</v>
+        <v>194</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>247</v>
+        <v>195</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>248</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -2229,52 +2241,52 @@
         <v>22</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>249</v>
+        <v>197</v>
       </c>
       <c r="F12" s="2">
         <v>1634882400</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>221</v>
+        <v>308</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>250</v>
+        <v>198</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>81</v>
+        <v>322</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>358</v>
+        <v>278</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>253</v>
+        <v>201</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>254</v>
+        <v>202</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>255</v>
+        <v>203</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>256</v>
+        <v>204</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>257</v>
+        <v>323</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>258</v>
+        <v>205</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>259</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -2291,52 +2303,52 @@
         <v>22</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>260</v>
+        <v>207</v>
       </c>
       <c r="F13" s="2">
         <v>1631858400</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>241</v>
+        <v>189</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>83</v>
+        <v>324</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>359</v>
+        <v>325</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>261</v>
+        <v>208</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>262</v>
+        <v>326</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>263</v>
+        <v>209</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>264</v>
+        <v>210</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>265</v>
+        <v>211</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>196</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -2353,52 +2365,52 @@
         <v>22</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>266</v>
+        <v>327</v>
       </c>
       <c r="F14" s="2">
         <v>1633068000</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>267</v>
+        <v>328</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>88</v>
+        <v>329</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>89</v>
+        <v>330</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>360</v>
+        <v>279</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>268</v>
+        <v>212</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>269</v>
+        <v>331</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>270</v>
+        <v>213</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>271</v>
+        <v>214</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>272</v>
+        <v>215</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>94</v>
+        <v>332</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -2415,52 +2427,52 @@
         <v>22</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="F15" s="2">
         <v>1634277600</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>160</v>
+        <v>129</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>273</v>
+        <v>216</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>361</v>
+        <v>280</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>97</v>
+        <v>333</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>98</v>
+        <v>334</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>274</v>
+        <v>335</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>275</v>
+        <v>336</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>276</v>
+        <v>217</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>277</v>
+        <v>218</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>278</v>
+        <v>219</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>279</v>
+        <v>220</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>280</v>
+        <v>337</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -2477,52 +2489,52 @@
         <v>22</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>281</v>
+        <v>338</v>
       </c>
       <c r="F16" s="2">
         <v>1634277600</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>160</v>
+        <v>129</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>282</v>
+        <v>221</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>283</v>
+        <v>222</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>362</v>
+        <v>281</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>284</v>
+        <v>339</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>285</v>
+        <v>223</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>286</v>
+        <v>224</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>287</v>
+        <v>340</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>288</v>
+        <v>225</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
@@ -2539,52 +2551,52 @@
         <v>22</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>105</v>
+        <v>341</v>
       </c>
       <c r="F17" s="2">
         <v>1642748400</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>289</v>
+        <v>226</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>50</v>
+        <v>290</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>290</v>
+        <v>342</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>363</v>
+        <v>282</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>291</v>
+        <v>227</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>292</v>
+        <v>228</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>293</v>
+        <v>229</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>294</v>
+        <v>230</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>295</v>
+        <v>231</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>296</v>
+        <v>232</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
@@ -2601,52 +2613,52 @@
         <v>22</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="F18" s="2">
         <v>1637305200</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>74</v>
+        <v>343</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>111</v>
+        <v>344</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>112</v>
+        <v>345</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>364</v>
+        <v>283</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>297</v>
+        <v>346</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>113</v>
+        <v>347</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>298</v>
+        <v>348</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>299</v>
+        <v>233</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>115</v>
+        <v>349</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>300</v>
+        <v>234</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>301</v>
+        <v>235</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
@@ -2663,52 +2675,52 @@
         <v>22</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>302</v>
+        <v>350</v>
       </c>
       <c r="F19" s="2">
         <v>1631253600</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>303</v>
+        <v>351</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>304</v>
+        <v>236</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>365</v>
+        <v>284</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>305</v>
+        <v>237</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>306</v>
+        <v>238</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>307</v>
+        <v>239</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>308</v>
+        <v>240</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>309</v>
+        <v>241</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>310</v>
+        <v>242</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>311</v>
+        <v>243</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
@@ -2725,52 +2737,52 @@
         <v>22</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>312</v>
+        <v>352</v>
       </c>
       <c r="F20" s="2">
         <v>1634882400</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>221</v>
+        <v>308</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>313</v>
+        <v>244</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>366</v>
+        <v>285</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>314</v>
+        <v>245</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>151</v>
+        <v>311</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>315</v>
+        <v>353</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>316</v>
+        <v>246</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>124</v>
+        <v>354</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>317</v>
+        <v>247</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>318</v>
+        <v>355</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
@@ -2787,52 +2799,52 @@
         <v>22</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>319</v>
+        <v>248</v>
       </c>
       <c r="F21" s="2">
         <v>1632463200</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>320</v>
+        <v>249</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>129</v>
+        <v>356</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>321</v>
+        <v>250</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>130</v>
+        <v>357</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>322</v>
+        <v>251</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>323</v>
+        <v>252</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>324</v>
+        <v>253</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>325</v>
+        <v>358</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>326</v>
+        <v>254</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>196</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
@@ -2849,52 +2861,52 @@
         <v>22</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="F22" s="2">
         <v>1649916000</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>133</v>
+        <v>359</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>327</v>
+        <v>360</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>367</v>
+        <v>286</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>328</v>
+        <v>255</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>329</v>
+        <v>361</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>330</v>
+        <v>256</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>135</v>
+        <v>110</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>331</v>
+        <v>257</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>332</v>
+        <v>362</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>333</v>
+        <v>363</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
@@ -2911,52 +2923,52 @@
         <v>22</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>138</v>
+        <v>364</v>
       </c>
       <c r="F23" s="2">
         <v>1631858400</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>334</v>
+        <v>365</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>335</v>
+        <v>258</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>336</v>
+        <v>259</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>337</v>
+        <v>260</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>338</v>
+        <v>366</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>339</v>
+        <v>261</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>340</v>
+        <v>262</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>140</v>
+        <v>367</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>341</v>
+        <v>263</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>342</v>
+        <v>368</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>343</v>
+        <v>264</v>
       </c>
       <c r="T23" s="2" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
@@ -2973,52 +2985,52 @@
         <v>22</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>344</v>
+        <v>265</v>
       </c>
       <c r="F24" s="2">
         <v>1631512800</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>142</v>
+        <v>115</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>345</v>
+        <v>266</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>145</v>
+        <v>118</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>346</v>
+        <v>267</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>146</v>
+        <v>369</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>347</v>
+        <v>268</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>348</v>
+        <v>269</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>349</v>
+        <v>270</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>147</v>
+        <v>370</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>148</v>
+        <v>119</v>
       </c>
       <c r="T24" s="2" t="s">
-        <v>351</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>

</xml_diff>